<commit_message>
changes in template again
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-CashDetailed-v3.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-CashDetailed-v3.xlsx
@@ -204,6 +204,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;#,##0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -245,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -407,47 +410,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -636,16 +598,113 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -654,9 +713,22 @@
       </left>
       <right/>
       <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -665,48 +737,8 @@
         <color auto="1"/>
       </right>
       <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -716,15 +748,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -739,121 +771,190 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -862,92 +963,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1228,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:N26"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1255,21 +1293,21 @@
       <c r="N1" s="6"/>
     </row>
     <row r="2" spans="2:14" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
@@ -1287,501 +1325,501 @@
       <c r="N3" s="6"/>
     </row>
     <row r="4" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="14"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="13"/>
     </row>
     <row r="5" spans="2:14" ht="13" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="18"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="2:14" ht="13" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="18"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="18"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="17"/>
     </row>
     <row r="8" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="18"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="17"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="18"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="17"/>
     </row>
     <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="17"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="18"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="19"/>
-      <c r="C12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="21"/>
-    </row>
-    <row r="13" spans="2:14" s="22" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="19"/>
-      <c r="C13" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="2:14" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="18"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="21"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="20"/>
     </row>
     <row r="14" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="23"/>
-      <c r="C14" s="17"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="26"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="25"/>
     </row>
     <row r="15" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="29" t="s">
+      <c r="L15" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="M15" s="29" t="s">
+      <c r="M15" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="30" t="s">
+      <c r="N15" s="29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="32" t="s">
+      <c r="I16" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="32" t="s">
+      <c r="J16" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="32" t="s">
+      <c r="K16" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="L16" s="32" t="s">
+      <c r="L16" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="32" t="s">
+      <c r="M16" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="N16" s="33" t="s">
+      <c r="N16" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="19"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="17"/>
     </row>
     <row r="18" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="36"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="65"/>
     </row>
     <row r="19" spans="2:14" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="39"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="68"/>
     </row>
     <row r="20" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43" t="s">
+      <c r="B20" s="53"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="44" t="s">
+      <c r="J20" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="44" t="s">
+      <c r="K20" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="L20" s="44" t="s">
+      <c r="L20" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="M20" s="44"/>
-      <c r="N20" s="45"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="36"/>
     </row>
     <row r="21" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="49" t="s">
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="J21" s="50"/>
-      <c r="K21" s="51" t="s">
+      <c r="J21" s="73"/>
+      <c r="K21" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="L21" s="52" t="s">
+      <c r="L21" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="M21" s="50"/>
-      <c r="N21" s="53"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="76"/>
     </row>
     <row r="22" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="54" t="s">
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="55"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="78"/>
+      <c r="M22" s="78"/>
+      <c r="N22" s="79"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="56"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="54"/>
     </row>
     <row r="24" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="59"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="57"/>
     </row>
     <row r="25" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="62" t="s">
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="63"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="62"/>
     </row>
     <row r="26" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="64" t="s">
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="65"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="65"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="66"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="51"/>
     </row>
     <row r="27" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="67" t="s">
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="55"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="45"/>
     </row>
     <row r="28" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="77"/>
-      <c r="D28" s="77"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="70" t="s">
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="68"/>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="68"/>
-      <c r="L28" s="68"/>
-      <c r="M28" s="68"/>
-      <c r="N28" s="71"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -1790,18 +1828,18 @@
     <mergeCell ref="B24:N24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="G25:N25"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="B18:N18"/>
+    <mergeCell ref="B19:N19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="G27:N27"/>
     <mergeCell ref="G28:N28"/>
     <mergeCell ref="G26:N26"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="B18:N18"/>
-    <mergeCell ref="B19:N19"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
More minor changes for invoice
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-CashDetailed-v3.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-CashDetailed-v3.xlsx
@@ -204,9 +204,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;₹&quot;#,##0"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -864,6 +861,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -894,15 +906,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -934,6 +937,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -963,28 +975,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1267,7 +1264,7 @@
   <dimension ref="B1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G26" sqref="G26:N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1293,21 +1290,21 @@
       <c r="N1" s="6"/>
     </row>
     <row r="2" spans="2:14" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
@@ -1615,46 +1612,46 @@
       <c r="N17" s="17"/>
     </row>
     <row r="18" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="64"/>
-      <c r="N18" s="65"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="70"/>
     </row>
     <row r="19" spans="2:14" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
-      <c r="N19" s="68"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="73"/>
     </row>
     <row r="20" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="53"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
       <c r="H20" s="33"/>
       <c r="I20" s="34" t="s">
         <v>15</v>
@@ -1672,154 +1669,154 @@
       <c r="N20" s="36"/>
     </row>
     <row r="21" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="69" t="s">
+      <c r="B21" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="72" t="s">
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="J21" s="73"/>
-      <c r="K21" s="74" t="s">
+      <c r="J21" s="40"/>
+      <c r="K21" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="L21" s="75" t="s">
+      <c r="L21" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="M21" s="73"/>
-      <c r="N21" s="76"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="43"/>
     </row>
     <row r="22" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="77" t="s">
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="78"/>
-      <c r="N22" s="79"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="67"/>
     </row>
     <row r="23" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="53"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="54"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="56"/>
     </row>
     <row r="24" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="57"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="59"/>
     </row>
     <row r="25" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
       <c r="E25" s="37"/>
       <c r="F25" s="37"/>
-      <c r="G25" s="60" t="s">
+      <c r="G25" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="62"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="64"/>
     </row>
     <row r="26" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="49" t="s">
+      <c r="G26" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="50"/>
-      <c r="N26" s="51"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="79"/>
     </row>
     <row r="27" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="43" t="s">
+      <c r="G27" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="45"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="50"/>
     </row>
     <row r="28" spans="2:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
-      <c r="G28" s="46" t="s">
+      <c r="G28" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="48"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>